<commit_message>
removed duplicated gold items
</commit_message>
<xml_diff>
--- a/everything.xlsx
+++ b/everything.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f43e12e3e204458/Documents/_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="412" documentId="8_{5BDF265E-2CF1-482D-A223-667A08E88109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{019A81DA-3E9B-4715-B090-1CAC65E11152}"/>
+  <xr:revisionPtr revIDLastSave="434" documentId="8_{5BDF265E-2CF1-482D-A223-667A08E88109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{651DE611-0433-4EA7-81ED-CF0342DCC259}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="630" xr2:uid="{A538EE8B-3260-45DE-98B8-1236EBB732D9}"/>
+    <workbookView xWindow="4770" yWindow="3840" windowWidth="28800" windowHeight="15345" tabRatio="630" activeTab="6" xr2:uid="{A538EE8B-3260-45DE-98B8-1236EBB732D9}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="8" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="1240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="1229">
   <si>
     <t>Allium</t>
   </si>
@@ -1732,46 +1732,13 @@
     <t>Goat spawn egg</t>
   </si>
   <si>
-    <t>Gold axe</t>
-  </si>
-  <si>
-    <t>Gold block</t>
-  </si>
-  <si>
-    <t>Gold boots</t>
-  </si>
-  <si>
-    <t>Gold chestplate</t>
-  </si>
-  <si>
-    <t>Gold helmet</t>
-  </si>
-  <si>
-    <t>Gold hoe</t>
-  </si>
-  <si>
-    <t>Gold horse armor</t>
-  </si>
-  <si>
     <t>Gold ingot</t>
   </si>
   <si>
-    <t>Gold leggings</t>
-  </si>
-  <si>
     <t>Gold nugget</t>
   </si>
   <si>
     <t>Gold ore</t>
-  </si>
-  <si>
-    <t>Gold pickaxe</t>
-  </si>
-  <si>
-    <t>Gold shovel</t>
-  </si>
-  <si>
-    <t>Gold sword</t>
   </si>
   <si>
     <t>Golden apple</t>
@@ -3824,7 +3791,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4517,8 +4504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C4D5B1-D50C-4F58-B25C-C0972980608D}">
   <dimension ref="A1:A34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A34"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4695,10 +4682,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A34">
-    <cfRule type="duplicateValues" dxfId="37" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A34">
-    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4716,17 +4703,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>662</v>
+        <v>651</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>663</v>
+        <v>652</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>664</v>
+        <v>653</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -4736,82 +4723,82 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>665</v>
+        <v>654</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>666</v>
+        <v>655</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>667</v>
+        <v>656</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>668</v>
+        <v>657</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>669</v>
+        <v>658</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>670</v>
+        <v>659</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>671</v>
+        <v>660</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>672</v>
+        <v>661</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>673</v>
+        <v>662</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>674</v>
+        <v>663</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>675</v>
+        <v>664</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>676</v>
+        <v>665</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>677</v>
+        <v>666</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>678</v>
+        <v>667</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>679</v>
+        <v>668</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A19">
-    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4832,12 +4819,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>680</v>
+        <v>669</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A2">
-    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4865,32 +4852,32 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>681</v>
+        <v>670</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>682</v>
+        <v>671</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>683</v>
+        <v>672</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>684</v>
+        <v>673</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>685</v>
+        <v>674</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>686</v>
+        <v>675</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -4905,42 +4892,42 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>688</v>
+        <v>677</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>689</v>
+        <v>678</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>690</v>
+        <v>679</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>691</v>
+        <v>680</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>692</v>
+        <v>681</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>693</v>
+        <v>682</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>694</v>
+        <v>683</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -4960,152 +4947,152 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>695</v>
+        <v>684</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>696</v>
+        <v>685</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>697</v>
+        <v>686</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>698</v>
+        <v>687</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>699</v>
+        <v>688</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>700</v>
+        <v>689</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>701</v>
+        <v>690</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>702</v>
+        <v>691</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>703</v>
+        <v>692</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>704</v>
+        <v>693</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>705</v>
+        <v>694</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>706</v>
+        <v>695</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>707</v>
+        <v>696</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>708</v>
+        <v>697</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>709</v>
+        <v>698</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>710</v>
+        <v>699</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>711</v>
+        <v>700</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>712</v>
+        <v>701</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>713</v>
+        <v>702</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>714</v>
+        <v>703</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>715</v>
+        <v>704</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>716</v>
+        <v>705</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>717</v>
+        <v>706</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>718</v>
+        <v>707</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>719</v>
+        <v>708</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>720</v>
+        <v>709</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>721</v>
+        <v>710</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>722</v>
+        <v>711</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>723</v>
+        <v>712</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>724</v>
+        <v>713</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
@@ -5115,102 +5102,102 @@
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>725</v>
+        <v>714</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>726</v>
+        <v>715</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>727</v>
+        <v>716</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>728</v>
+        <v>717</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>729</v>
+        <v>718</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>730</v>
+        <v>719</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>731</v>
+        <v>720</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>732</v>
+        <v>721</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>733</v>
+        <v>722</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>734</v>
+        <v>723</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>735</v>
+        <v>724</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>736</v>
+        <v>725</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>737</v>
+        <v>726</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>738</v>
+        <v>727</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>739</v>
+        <v>728</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>740</v>
+        <v>729</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>741</v>
+        <v>730</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>742</v>
+        <v>731</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>743</v>
+        <v>732</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>744</v>
+        <v>733</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
@@ -5220,7 +5207,7 @@
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>745</v>
+        <v>734</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
@@ -5230,7 +5217,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A53">
-    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5248,82 +5235,82 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>746</v>
+        <v>735</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>747</v>
+        <v>736</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>748</v>
+        <v>737</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>749</v>
+        <v>738</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>750</v>
+        <v>739</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>751</v>
+        <v>740</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>752</v>
+        <v>741</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>753</v>
+        <v>742</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>754</v>
+        <v>743</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>755</v>
+        <v>744</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>756</v>
+        <v>745</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>757</v>
+        <v>746</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>758</v>
+        <v>747</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>759</v>
+        <v>748</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>760</v>
+        <v>749</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>761</v>
+        <v>750</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -5333,7 +5320,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>762</v>
+        <v>751</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -5343,27 +5330,27 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>763</v>
+        <v>752</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>764</v>
+        <v>753</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>765</v>
+        <v>754</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>766</v>
+        <v>755</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
@@ -5373,132 +5360,132 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>768</v>
+        <v>757</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>770</v>
+        <v>759</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>771</v>
+        <v>760</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>772</v>
+        <v>761</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>773</v>
+        <v>762</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>774</v>
+        <v>763</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>775</v>
+        <v>764</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>776</v>
+        <v>765</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>777</v>
+        <v>766</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>778</v>
+        <v>767</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>779</v>
+        <v>768</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>780</v>
+        <v>769</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>781</v>
+        <v>770</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>782</v>
+        <v>771</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>783</v>
+        <v>772</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>784</v>
+        <v>773</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>785</v>
+        <v>774</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>786</v>
+        <v>775</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>787</v>
+        <v>776</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>788</v>
+        <v>777</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>789</v>
+        <v>778</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>790</v>
+        <v>779</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>791</v>
+        <v>780</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>792</v>
+        <v>781</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>793</v>
+        <v>782</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
@@ -5523,137 +5510,137 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>794</v>
+        <v>783</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>795</v>
+        <v>784</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>796</v>
+        <v>785</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>797</v>
+        <v>786</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>798</v>
+        <v>787</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>799</v>
+        <v>788</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>800</v>
+        <v>789</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>801</v>
+        <v>790</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>802</v>
+        <v>791</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>803</v>
+        <v>792</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>804</v>
+        <v>793</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>805</v>
+        <v>794</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>806</v>
+        <v>795</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>807</v>
+        <v>796</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>808</v>
+        <v>797</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>809</v>
+        <v>798</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>810</v>
+        <v>799</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>811</v>
+        <v>800</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>812</v>
+        <v>801</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>813</v>
+        <v>802</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>814</v>
+        <v>803</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>815</v>
+        <v>804</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>816</v>
+        <v>805</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>817</v>
+        <v>806</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>818</v>
+        <v>807</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>819</v>
+        <v>808</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>820</v>
+        <v>809</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
@@ -5663,7 +5650,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>821</v>
+        <v>810</v>
       </c>
     </row>
   </sheetData>
@@ -5683,82 +5670,82 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>822</v>
+        <v>811</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>823</v>
+        <v>812</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>824</v>
+        <v>813</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>825</v>
+        <v>814</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>826</v>
+        <v>815</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>827</v>
+        <v>816</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>828</v>
+        <v>817</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>829</v>
+        <v>818</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>830</v>
+        <v>819</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>831</v>
+        <v>820</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>832</v>
+        <v>821</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>833</v>
+        <v>822</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>834</v>
+        <v>823</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>835</v>
+        <v>824</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>836</v>
+        <v>825</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>837</v>
+        <v>826</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -5773,102 +5760,102 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>838</v>
+        <v>827</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>839</v>
+        <v>828</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>840</v>
+        <v>829</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>841</v>
+        <v>830</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>842</v>
+        <v>831</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>843</v>
+        <v>832</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>844</v>
+        <v>833</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>845</v>
+        <v>834</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>846</v>
+        <v>835</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>847</v>
+        <v>836</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>848</v>
+        <v>837</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>849</v>
+        <v>838</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>850</v>
+        <v>839</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>851</v>
+        <v>840</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>852</v>
+        <v>841</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>853</v>
+        <v>842</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>854</v>
+        <v>843</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>855</v>
+        <v>844</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>856</v>
+        <v>845</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>857</v>
+        <v>846</v>
       </c>
     </row>
   </sheetData>
@@ -5888,7 +5875,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>858</v>
+        <v>847</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -5908,92 +5895,92 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>859</v>
+        <v>848</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>860</v>
+        <v>849</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>861</v>
+        <v>850</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>862</v>
+        <v>851</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>863</v>
+        <v>852</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>864</v>
+        <v>853</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>865</v>
+        <v>854</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>866</v>
+        <v>855</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>867</v>
+        <v>856</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>868</v>
+        <v>857</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>869</v>
+        <v>858</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>870</v>
+        <v>859</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>871</v>
+        <v>860</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>872</v>
+        <v>861</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>873</v>
+        <v>862</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>874</v>
+        <v>863</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>875</v>
+        <v>864</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>876</v>
+        <v>865</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -6003,17 +5990,17 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>877</v>
+        <v>866</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>878</v>
+        <v>867</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>879</v>
+        <v>868</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
@@ -6023,167 +6010,167 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>880</v>
+        <v>869</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>881</v>
+        <v>870</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>882</v>
+        <v>871</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>883</v>
+        <v>872</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>884</v>
+        <v>873</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>885</v>
+        <v>874</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>886</v>
+        <v>875</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>887</v>
+        <v>876</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>888</v>
+        <v>877</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>889</v>
+        <v>878</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>890</v>
+        <v>879</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>891</v>
+        <v>880</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>892</v>
+        <v>881</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>893</v>
+        <v>882</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>894</v>
+        <v>883</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>895</v>
+        <v>884</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>896</v>
+        <v>885</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>897</v>
+        <v>886</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>898</v>
+        <v>887</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>899</v>
+        <v>888</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>900</v>
+        <v>889</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>901</v>
+        <v>890</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>902</v>
+        <v>891</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>903</v>
+        <v>892</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>904</v>
+        <v>893</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>905</v>
+        <v>894</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>906</v>
+        <v>895</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>907</v>
+        <v>896</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>908</v>
+        <v>897</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>909</v>
+        <v>898</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>910</v>
+        <v>899</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>911</v>
+        <v>900</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>912</v>
+        <v>901</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
@@ -6208,22 +6195,22 @@
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>913</v>
+        <v>902</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>914</v>
+        <v>903</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>915</v>
+        <v>904</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>916</v>
+        <v>905</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
@@ -6233,42 +6220,42 @@
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>917</v>
+        <v>906</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>918</v>
+        <v>907</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>919</v>
+        <v>908</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>920</v>
+        <v>909</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>921</v>
+        <v>910</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>922</v>
+        <v>911</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>923</v>
+        <v>912</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>924</v>
+        <v>913</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
@@ -6283,123 +6270,123 @@
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>925</v>
+        <v>914</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>926</v>
+        <v>915</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>927</v>
+        <v>916</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>928</v>
+        <v>917</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>929</v>
+        <v>918</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>930</v>
+        <v>919</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>931</v>
+        <v>920</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>932</v>
+        <v>921</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>933</v>
+        <v>922</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>934</v>
+        <v>923</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>935</v>
+        <v>924</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>936</v>
+        <v>925</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>937</v>
+        <v>926</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>938</v>
+        <v>927</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>939</v>
+        <v>928</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>940</v>
+        <v>929</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>941</v>
+        <v>930</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>942</v>
+        <v>931</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>943</v>
+        <v>932</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>944</v>
+        <v>933</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>945</v>
+        <v>934</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>946</v>
+        <v>935</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A75:A102">
-    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A75:A102">
-    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A75:A102">
-    <cfRule type="duplicateValues" dxfId="14" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6417,38 +6404,38 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>947</v>
+        <v>936</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>948</v>
+        <v>937</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>949</v>
+        <v>938</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>950</v>
+        <v>939</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>951</v>
+        <v>940</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A5">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A5">
-    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A5">
-    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6469,17 +6456,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>952</v>
+        <v>941</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>953</v>
+        <v>942</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>954</v>
+        <v>943</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -6489,187 +6476,187 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>955</v>
+        <v>944</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>956</v>
+        <v>945</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>957</v>
+        <v>946</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>958</v>
+        <v>947</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>959</v>
+        <v>948</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>960</v>
+        <v>949</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>961</v>
+        <v>950</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>962</v>
+        <v>951</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>963</v>
+        <v>952</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>964</v>
+        <v>953</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>965</v>
+        <v>954</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>966</v>
+        <v>955</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>967</v>
+        <v>956</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>968</v>
+        <v>957</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>969</v>
+        <v>958</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>970</v>
+        <v>959</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>971</v>
+        <v>960</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>972</v>
+        <v>961</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>973</v>
+        <v>962</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>974</v>
+        <v>963</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>975</v>
+        <v>964</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>976</v>
+        <v>965</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>977</v>
+        <v>966</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>978</v>
+        <v>967</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>979</v>
+        <v>968</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>980</v>
+        <v>969</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>981</v>
+        <v>970</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>982</v>
+        <v>971</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>983</v>
+        <v>972</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>984</v>
+        <v>973</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>985</v>
+        <v>974</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>986</v>
+        <v>975</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>987</v>
+        <v>976</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>988</v>
+        <v>977</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>989</v>
+        <v>978</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>990</v>
+        <v>979</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>991</v>
+        <v>980</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -6679,109 +6666,109 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>992</v>
+        <v>981</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>993</v>
+        <v>982</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>994</v>
+        <v>983</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>995</v>
+        <v>984</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>996</v>
+        <v>985</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>997</v>
+        <v>986</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>998</v>
+        <v>987</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>999</v>
+        <v>988</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1000</v>
+        <v>989</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1001</v>
+        <v>990</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1002</v>
+        <v>991</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1003</v>
+        <v>992</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1004</v>
+        <v>993</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1005</v>
+        <v>994</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1006</v>
+        <v>995</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1007</v>
+        <v>996</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1008</v>
+        <v>997</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1009</v>
+        <v>998</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A38:A57 A1:A35">
-    <cfRule type="duplicateValues" dxfId="10" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:A57 A1:A35">
-    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:A57 A1:A35">
-    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69:A71">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6814,17 +6801,17 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1010</v>
+        <v>999</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1011</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1012</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
@@ -6834,7 +6821,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1013</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -6844,12 +6831,12 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1014</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1015</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -6874,12 +6861,12 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1016</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1017</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -6889,7 +6876,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1018</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
@@ -6899,7 +6886,7 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1019</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -6909,37 +6896,37 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1020</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1021</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1022</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1023</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1024</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1025</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1026</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
@@ -6949,62 +6936,62 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1027</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1028</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1029</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1030</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1031</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1032</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1033</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1034</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1035</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1036</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1037</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1038</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
@@ -7014,12 +7001,12 @@
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1039</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1040</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
@@ -7029,147 +7016,147 @@
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1041</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1042</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1043</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1044</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1045</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1046</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1047</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1048</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1049</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1050</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1051</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1052</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1053</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1054</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1055</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1056</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1057</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>1058</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>1059</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>1060</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>1061</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>1062</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>1063</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>1064</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>1065</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>1066</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>1067</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>1068</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>1069</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
@@ -7179,17 +7166,17 @@
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>1070</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>1071</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>1072</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
@@ -7199,87 +7186,87 @@
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>1073</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>1074</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>1075</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>1076</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>1077</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>1078</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>1079</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>1080</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>1081</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>1082</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>1083</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>1084</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>1085</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>1086</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>1087</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>1088</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>1089</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
@@ -7289,7 +7276,7 @@
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>1090</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
@@ -7304,7 +7291,7 @@
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>1091</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
@@ -7314,87 +7301,87 @@
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>1092</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>1093</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>1094</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>1095</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>1096</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>1097</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>1098</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>1099</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>1100</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>1101</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>1102</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>1103</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>1104</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>1105</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>1106</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>1107</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>1108</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
@@ -7404,32 +7391,32 @@
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>1109</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>1110</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>1111</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>1112</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>1113</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>1114</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
@@ -7439,82 +7426,82 @@
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>1115</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>1116</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>1117</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>1118</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>1119</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>1120</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>1121</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>1122</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>1123</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>1124</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>1125</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>1126</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>1127</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>1128</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>1129</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>1130</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
@@ -7524,7 +7511,7 @@
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>1131</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
@@ -7544,53 +7531,53 @@
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>1132</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>1133</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>1134</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>1135</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>1136</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>1137</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>1138</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>1139</v>
+        <v>1128</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A30">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A12 A121:A157">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65:A157 A58:A60 A7:A54">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7600,8 +7587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F35CFE-21C5-453C-B2F2-17B7AD9D64B4}">
   <dimension ref="A1:A127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A127"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A34" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8243,10 +8230,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A127">
-    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A127">
-    <cfRule type="duplicateValues" dxfId="34" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8264,7 +8254,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1140</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -8279,17 +8269,17 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1141</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1142</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1143</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
@@ -8304,7 +8294,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1144</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -8314,7 +8304,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1145</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -8329,27 +8319,27 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1146</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1147</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1148</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1149</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1150</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -8359,22 +8349,22 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1151</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1152</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1153</v>
+        <v>1142</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A22">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8407,7 +8397,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8425,92 +8415,92 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1154</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1155</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1156</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1157</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1158</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1159</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1160</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1161</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1162</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1163</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1164</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1165</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1166</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1167</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1168</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1169</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1170</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -8520,117 +8510,117 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1173</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1174</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1175</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1176</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1177</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1178</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1179</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1180</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1181</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1182</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1183</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1184</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1185</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1186</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1187</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1188</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1189</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1190</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1191</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1192</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1193</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1194</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
@@ -8640,12 +8630,12 @@
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1195</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1196</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
@@ -8655,152 +8645,152 @@
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1197</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1198</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1199</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1200</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1201</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1202</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1203</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1204</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1205</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1206</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1207</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1208</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1209</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1210</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1211</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1212</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1213</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>1214</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>1215</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>1216</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>1217</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>1218</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>1219</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>1220</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>1221</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>1222</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>1223</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>1224</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>1225</v>
+        <v>1214</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A75">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8830,72 +8820,72 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1226</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1227</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1228</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1229</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1230</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1231</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1232</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1233</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1234</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1235</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1236</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1237</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1238</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1239</v>
+        <v>1228</v>
       </c>
     </row>
   </sheetData>
@@ -8920,7 +8910,7 @@
   <dimension ref="A1:A116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A116"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9507,10 +9497,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A116">
-    <cfRule type="duplicateValues" dxfId="33" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A116">
-    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9521,7 +9511,7 @@
   <dimension ref="A1:A125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A125"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10153,10 +10143,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A125">
-    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A125">
-    <cfRule type="duplicateValues" dxfId="30" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10167,7 +10157,7 @@
   <dimension ref="A1:A39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A39"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10369,10 +10359,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A39">
-    <cfRule type="duplicateValues" dxfId="29" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A39">
-    <cfRule type="duplicateValues" dxfId="28" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10495,10 +10485,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A21">
-    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A21">
-    <cfRule type="duplicateValues" dxfId="26" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10506,10 +10496,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82B99E7A-ECFE-42AC-BE3E-B3428AB86D0B}">
-  <dimension ref="A1:A79"/>
+  <dimension ref="A1:A68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10666,97 +10656,97 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>572</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>576</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>579</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>580</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>584</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>587</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
@@ -10846,75 +10836,20 @@
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>605</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A79">
-    <cfRule type="duplicateValues" dxfId="25" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A79">
-    <cfRule type="duplicateValues" dxfId="24" priority="2"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A71">
+    <sortCondition ref="A7:A71"/>
+  </sortState>
+  <conditionalFormatting sqref="A73 A1:A69">
+    <cfRule type="duplicateValues" dxfId="29" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10932,77 +10867,77 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>616</v>
+        <v>605</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>617</v>
+        <v>606</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>619</v>
+        <v>608</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>620</v>
+        <v>609</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>621</v>
+        <v>610</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>622</v>
+        <v>611</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>623</v>
+        <v>612</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>624</v>
+        <v>613</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>625</v>
+        <v>614</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>626</v>
+        <v>615</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>627</v>
+        <v>616</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>628</v>
+        <v>617</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>629</v>
+        <v>618</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>630</v>
+        <v>619</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
@@ -11012,7 +10947,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>631</v>
+        <v>620</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -11022,28 +10957,28 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>632</v>
+        <v>621</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>633</v>
+        <v>622</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>634</v>
+        <v>623</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:A21">
-    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A3">
-    <cfRule type="duplicateValues" dxfId="22" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A3">
-    <cfRule type="duplicateValues" dxfId="21" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11066,142 +11001,142 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>635</v>
+        <v>624</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>636</v>
+        <v>625</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>637</v>
+        <v>626</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>638</v>
+        <v>627</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>639</v>
+        <v>628</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>640</v>
+        <v>629</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>641</v>
+        <v>630</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>642</v>
+        <v>631</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>644</v>
+        <v>633</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>645</v>
+        <v>634</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>646</v>
+        <v>635</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>647</v>
+        <v>636</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>648</v>
+        <v>637</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>649</v>
+        <v>638</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>650</v>
+        <v>639</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>651</v>
+        <v>640</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>652</v>
+        <v>641</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>653</v>
+        <v>642</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>654</v>
+        <v>643</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>655</v>
+        <v>644</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>656</v>
+        <v>645</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>657</v>
+        <v>646</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>658</v>
+        <v>647</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>659</v>
+        <v>648</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>660</v>
+        <v>649</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>661</v>
+        <v>650</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A28">
-    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>